<commit_message>
🐛Arreglar los archivos de lectura
</commit_message>
<xml_diff>
--- a/recursos/Emparejamiento.xlsx
+++ b/recursos/Emparejamiento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3E6AA3-2B6E-44A7-AB4D-184F4CBC6F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601A1D1B-B33E-4718-B6EA-F074C2B9B121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="670" xr2:uid="{FD9F6918-DD5F-4EFB-A5DA-81B3D2DC95CD}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="146">
   <si>
     <t>1.id</t>
   </si>
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t>Yulipati2011@hotmail.com</t>
-  </si>
-  <si>
-    <t>Modalidad 80 horas - 1 solo tutorado</t>
   </si>
   <si>
     <t xml:space="preserve">Ilian David </t>
@@ -281,9 +278,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Virtual</t>
-  </si>
-  <si>
     <t>Miguel EsparzaT</t>
   </si>
   <si>
@@ -344,9 +338,6 @@
     <t>Colegio Especial</t>
   </si>
   <si>
-    <t>santiago.diaz@javeriana.edu.co</t>
-  </si>
-  <si>
     <t>Andrea</t>
   </si>
   <si>
@@ -501,6 +492,18 @@
   </si>
   <si>
     <t>Colegio San Agustin</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Prueba3@pruebmail.com</t>
   </si>
 </sst>
 </file>
@@ -2004,8 +2007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D120C5C-D1E3-40C4-B4D7-C7D7020D0451}">
   <dimension ref="A1:AU57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,43 +2163,43 @@
         <v>44</v>
       </c>
       <c r="AU1" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:47" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="I2" s="16">
         <v>20</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K2" s="18">
         <v>1000477320</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M2" s="17">
         <v>3058829527</v>
@@ -2205,7 +2208,7 @@
         <v>3498597548</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P2" s="17"/>
       <c r="Q2" s="29">
@@ -2242,13 +2245,13 @@
         <v>3.1</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AC2" s="18">
         <v>1010944104</v>
       </c>
       <c r="AD2" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AE2" s="17">
         <v>3045124420</v>
@@ -2257,7 +2260,7 @@
         <v>3032568220</v>
       </c>
       <c r="AG2" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AH2" s="17"/>
       <c r="AI2" s="29">
@@ -2294,46 +2297,46 @@
         <v>3.2</v>
       </c>
       <c r="AT2" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AU2" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:47" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="E3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="15" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K3" s="6">
         <v>1037883695</v>
       </c>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M3">
         <v>3117565623</v>
@@ -2342,54 +2345,54 @@
         <v>3113735209</v>
       </c>
       <c r="O3" s="30" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Q3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="R3" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S3" s="28">
         <f t="shared" ref="S3:AA10" ca="1" si="0">ROUND(RAND()*5,1)</f>
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="T3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>1.9</v>
       </c>
       <c r="U3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>4.8</v>
       </c>
       <c r="V3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>5</v>
       </c>
       <c r="W3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="X3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="Y3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
+        <v>3.3</v>
       </c>
       <c r="Z3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="AA3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>3.1</v>
       </c>
       <c r="AB3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AC3">
         <v>1023456789</v>
@@ -2403,89 +2406,89 @@
       <c r="AG3" s="30"/>
       <c r="AI3">
         <f t="shared" ref="AI3:AS8" ca="1" si="1">ROUND(RAND()*5,1)</f>
+        <v>2</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.1</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" ca="1" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="AJ3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AL3">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.7</v>
-      </c>
-      <c r="AM3">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.3</v>
-      </c>
       <c r="AN3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
+        <v>0.2</v>
       </c>
       <c r="AO3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
       <c r="AP3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="AQ3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3</v>
+        <v>0.2</v>
       </c>
       <c r="AR3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="AS3">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3</v>
+        <v>1.2</v>
       </c>
       <c r="AT3" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AU3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:47" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="15" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K4" s="6">
         <v>1040872361</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M4">
         <v>3244716820</v>
@@ -2494,54 +2497,54 @@
         <v>3146538937</v>
       </c>
       <c r="O4" s="30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="28">
         <f ca="1">ROUND(RAND()*5,1)</f>
-        <v>1.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R4" s="28">
         <f t="shared" ref="R4:R10" ca="1" si="2">ROUND(RAND()*5,1)</f>
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="S4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="T4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>1.2</v>
       </c>
       <c r="U4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
+        <v>4.5</v>
       </c>
       <c r="V4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="W4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="X4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>3.3</v>
       </c>
       <c r="Y4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Z4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="AA4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="AB4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AC4">
         <v>1122334455</v>
@@ -2555,89 +2558,89 @@
       <c r="AG4" s="30"/>
       <c r="AI4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8</v>
+        <v>3.5</v>
       </c>
       <c r="AJ4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AK4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="AL4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="AM4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AN4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3</v>
+        <v>2.5</v>
       </c>
       <c r="AO4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>3.7</v>
       </c>
       <c r="AP4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AQ4">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="AR4">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6</v>
+        <v>3.1</v>
       </c>
       <c r="AS4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
+        <v>3.9</v>
       </c>
       <c r="AT4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AU4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:47" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="15" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K5">
         <v>1040334221</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M5">
         <v>3107589894</v>
@@ -2646,54 +2649,54 @@
         <v>3025791188</v>
       </c>
       <c r="O5" s="30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="Q5" s="28">
         <f t="shared" ref="Q5:Q10" ca="1" si="3">ROUND(RAND()*5,1)</f>
-        <v>0.5</v>
+        <v>1.6</v>
       </c>
       <c r="R5" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9</v>
+        <v>1.3</v>
       </c>
       <c r="S5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>3.9</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
       <c r="U5" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V5" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="V5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
-      </c>
       <c r="W5" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="X5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="Y5" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="Z5" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="X5" s="28">
+      <c r="AA5" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="Y5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.8</v>
-      </c>
-      <c r="Z5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7</v>
-      </c>
-      <c r="AA5" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
-      </c>
       <c r="AB5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AC5">
         <v>1234567890</v>
@@ -2706,31 +2709,31 @@
       </c>
       <c r="AI5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="AJ5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
       <c r="AK5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2</v>
+        <v>4.3</v>
       </c>
       <c r="AL5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="AM5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5</v>
+        <v>1.4</v>
       </c>
       <c r="AN5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="AO5">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="AP5">
         <f t="shared" ca="1" si="1"/>
@@ -2738,57 +2741,57 @@
       </c>
       <c r="AQ5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8</v>
+        <v>0.9</v>
       </c>
       <c r="AR5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
+        <v>3.7</v>
       </c>
       <c r="AS5">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3</v>
+        <v>4.8</v>
       </c>
       <c r="AT5" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AU5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:47" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="C6" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="15" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K6" s="6">
         <v>1046716109</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M6">
         <v>3243098774</v>
@@ -2797,55 +2800,55 @@
         <v>3044155979</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="P6" s="17"/>
       <c r="Q6" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8</v>
+        <v>1.3</v>
       </c>
       <c r="R6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2999999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="S6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>2.5</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="U6" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="V6" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="W6" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="U6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
-      </c>
-      <c r="V6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
-      </c>
-      <c r="W6" s="28">
+      <c r="X6" s="28">
         <f t="shared" ca="1" si="0"/>
         <v>4.7</v>
       </c>
-      <c r="X6" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
       <c r="Y6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
+        <v>0.7</v>
       </c>
       <c r="Z6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>1.8</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="AB6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AC6" s="18">
         <v>1098765432</v>
@@ -2861,89 +2864,89 @@
       <c r="AH6" s="17"/>
       <c r="AI6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
       <c r="AJ6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="AK6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9</v>
+        <v>5</v>
       </c>
       <c r="AL6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AM6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="AN6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7</v>
+        <v>3.1</v>
       </c>
       <c r="AO6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="AP6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
+        <v>3.2</v>
       </c>
       <c r="AQ6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AR6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>1.3</v>
       </c>
       <c r="AS6" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="AT6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AU6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:47" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="15" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K7" s="6">
         <v>1020316404</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M7">
         <v>3225962995</v>
@@ -2952,54 +2955,54 @@
         <v>3105528456</v>
       </c>
       <c r="O7" s="30" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2</v>
+        <v>2.5</v>
       </c>
       <c r="R7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8</v>
+        <v>3.6</v>
       </c>
       <c r="S7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>0.9</v>
       </c>
       <c r="T7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6</v>
+        <v>1.7</v>
       </c>
       <c r="U7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>2.7</v>
       </c>
       <c r="V7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="W7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
+        <v>0.9</v>
       </c>
       <c r="X7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>4.7</v>
       </c>
       <c r="Y7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>0.4</v>
       </c>
       <c r="Z7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
+        <v>1.9</v>
       </c>
       <c r="AA7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="AB7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AE7">
         <v>3216677889</v>
@@ -3009,89 +3012,89 @@
       </c>
       <c r="AI7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
+        <v>0.8</v>
       </c>
       <c r="AJ7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7</v>
+        <v>1.3</v>
       </c>
       <c r="AK7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>2.7</v>
       </c>
       <c r="AL7">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1</v>
+        <v>0.5</v>
       </c>
       <c r="AM7">
         <f t="shared" ca="1" si="1"/>
+        <v>2.7</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="AQ7">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.9</v>
+      </c>
+      <c r="AR7">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.4</v>
+      </c>
+      <c r="AS7">
+        <f t="shared" ca="1" si="1"/>
         <v>2.8</v>
       </c>
-      <c r="AN7">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="AO7">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="AP7">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="AQ7">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AR7">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="AS7">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.5999999999999996</v>
-      </c>
       <c r="AT7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AU7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:47" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="E8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="15" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K8" s="6">
         <v>1137725488</v>
       </c>
       <c r="L8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M8">
         <v>3294344455</v>
@@ -3100,54 +3103,54 @@
         <v>3284344455</v>
       </c>
       <c r="O8" s="30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q8" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="R8" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="S8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3</v>
+        <v>2.4</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8</v>
+        <v>3.9</v>
       </c>
       <c r="U8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>3.6</v>
       </c>
       <c r="V8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="W8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="X8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2</v>
+        <v>2.4</v>
       </c>
       <c r="Y8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7</v>
+        <v>2.8</v>
       </c>
       <c r="Z8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="AA8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>3.7</v>
       </c>
       <c r="AB8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AE8">
         <v>3237788990</v>
@@ -3157,89 +3160,89 @@
       </c>
       <c r="AI8">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AJ8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>1.7</v>
       </c>
       <c r="AK8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8</v>
+        <v>2.1</v>
       </c>
       <c r="AL8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1</v>
+        <v>2.5</v>
       </c>
       <c r="AM8">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>1.3</v>
       </c>
       <c r="AN8">
         <f t="shared" ca="1" si="1"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AO8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7</v>
+      </c>
+      <c r="AP8">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AQ8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="AR8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7</v>
+      </c>
+      <c r="AS8">
+        <f t="shared" ca="1" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="AO8">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="AP8">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="AQ8">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.4</v>
-      </c>
-      <c r="AR8">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
-      </c>
-      <c r="AS8">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.5</v>
-      </c>
       <c r="AT8" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AU8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:47" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="15" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K9" s="6">
         <v>1070753987</v>
       </c>
       <c r="L9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M9">
         <v>3262122233</v>
@@ -3248,82 +3251,82 @@
         <v>3295455566</v>
       </c>
       <c r="O9" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q9" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="R9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.4</v>
+        <v>1.9</v>
       </c>
       <c r="S9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="T9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>1.3</v>
       </c>
       <c r="U9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
+        <v>2.7</v>
       </c>
       <c r="W9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="X9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="Y9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>3.7</v>
       </c>
       <c r="Z9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>3.6</v>
       </c>
       <c r="AA9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
+        <v>4.7</v>
       </c>
       <c r="AT9" s="7"/>
     </row>
     <row r="10" spans="1:47" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>114</v>
-      </c>
       <c r="E10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K10" s="6">
         <v>1070653287</v>
@@ -3335,69 +3338,69 @@
         <v>3251011123</v>
       </c>
       <c r="O10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Q10" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="R10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5</v>
+        <v>1.7</v>
       </c>
       <c r="S10" s="28">
         <f t="shared" ca="1" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="T10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="U10" s="28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="V10" s="28">
+        <f t="shared" ca="1" si="0"/>
         <v>2.9</v>
       </c>
-      <c r="T10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="U10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="V10" s="28">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.3</v>
-      </c>
       <c r="W10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="X10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>3.2</v>
       </c>
       <c r="Y10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4</v>
+        <v>0.9</v>
       </c>
       <c r="Z10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
       <c r="AT10" s="7"/>
     </row>
-    <row r="11" spans="1:47" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>47</v>
@@ -3406,13 +3409,13 @@
         <v>46</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K11" s="6">
         <v>1044655071</v>

</xml_diff>

<commit_message>
emparejamiento corregido  a falta de modalidad
</commit_message>
<xml_diff>
--- a/recursos/Emparejamiento.xlsx
+++ b/recursos/Emparejamiento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darve\OneDrive\Documentos\GitHub\tugestor\Sistema-TuGestor\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64050EA5-53E4-4DD6-B102-51C4DD866967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00AB323-0294-447B-AFB2-4CD4991CAB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{E4CE6423-A843-4628-8D07-08B243EE4D92}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="87">
   <si>
     <t>nom tutor</t>
   </si>
@@ -280,6 +280,24 @@
   </si>
   <si>
     <t>34 horas horas</t>
+  </si>
+  <si>
+    <t>Ingles</t>
+  </si>
+  <si>
+    <t>mañana</t>
+  </si>
+  <si>
+    <t>gmail</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>mama</t>
+  </si>
+  <si>
+    <t>papa</t>
   </si>
 </sst>
 </file>
@@ -1703,14 +1721,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7378BA-084B-468C-A1CA-4BB48C8C069A}">
   <dimension ref="A1:AX13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="9" max="9" width="35.81640625" customWidth="1"/>
     <col min="10" max="10" width="25.453125" customWidth="1"/>
+    <col min="29" max="29" width="28.90625" customWidth="1"/>
+    <col min="30" max="30" width="24.1796875" customWidth="1"/>
+    <col min="49" max="49" width="47.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="39" x14ac:dyDescent="0.35">
@@ -1872,6 +1893,12 @@
       <c r="B2" t="s">
         <v>61</v>
       </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2">
+        <v>1234</v>
+      </c>
       <c r="G2" t="s">
         <v>58</v>
       </c>
@@ -1890,23 +1917,47 @@
       <c r="L2">
         <v>1</v>
       </c>
+      <c r="N2">
+        <v>123</v>
+      </c>
+      <c r="O2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" t="s">
+        <v>85</v>
+      </c>
       <c r="Q2" t="s">
         <v>57</v>
       </c>
       <c r="AC2" t="s">
         <v>66</v>
       </c>
+      <c r="AD2" t="s">
+        <v>82</v>
+      </c>
       <c r="AE2" t="s">
         <v>54</v>
       </c>
       <c r="AF2">
         <v>3</v>
       </c>
+      <c r="AH2">
+        <v>123</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>86</v>
+      </c>
       <c r="AK2" t="s">
         <v>62</v>
       </c>
       <c r="AW2" t="s">
         <v>59</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.35">
@@ -1917,7 +1968,7 @@
         <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="H3" t="s">
         <v>77</v>

</xml_diff>